<commit_message>
Actualización 1 de agosto de 2023 - Lap HP
Se actualiza el repositorio con materiales para el tercer examen parcial.
</commit_message>
<xml_diff>
--- a/Combinacion/Bitacora_Fisica_1_NRC_240_Segundo_Parcial.xlsx
+++ b/Combinacion/Bitacora_Fisica_1_NRC_240_Segundo_Parcial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Cuatrimestral\Fisica_1_BC\Combinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4384094-7182-4E52-BFF4-43318DCAAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5A5DC8-986A-44B9-B5A7-2C6F79D2A883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{977847BF-1F15-48C1-8F78-06C8B84025CC}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="219">
   <si>
     <t>Matrícula</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>Faltas</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -4933,11 +4936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282BE024-4F4F-468F-BFFD-FBEB26858532}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5031,7 +5033,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="2" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -5104,7 +5106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5178,7 +5180,7 @@
         <v>8.0333333333333332</v>
       </c>
     </row>
-    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -5252,7 +5254,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -5326,7 +5328,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -5400,7 +5402,7 @@
         <v>10.033333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -5474,7 +5476,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -5548,7 +5550,7 @@
         <v>8.0333333333333332</v>
       </c>
     </row>
-    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -5622,7 +5624,7 @@
         <v>9.3666666666666671</v>
       </c>
     </row>
-    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -5770,7 +5772,7 @@
         <v>6.0333333333333332</v>
       </c>
     </row>
-    <row r="12" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -5844,7 +5846,7 @@
         <v>9.3666666666666671</v>
       </c>
     </row>
-    <row r="13" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -5918,7 +5920,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -5992,7 +5994,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -6066,7 +6068,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -6140,7 +6142,7 @@
         <v>6.0333333333333332</v>
       </c>
     </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -6214,7 +6216,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -6288,7 +6290,7 @@
         <v>9.3666666666666671</v>
       </c>
     </row>
-    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -6362,7 +6364,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -6436,7 +6438,7 @@
         <v>10.033333333333333</v>
       </c>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -6510,7 +6512,7 @@
         <v>10.033333333333333</v>
       </c>
     </row>
-    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -6584,7 +6586,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -6658,7 +6660,7 @@
         <v>10.033333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -6732,7 +6734,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -6806,7 +6808,7 @@
         <v>8.0333333333333332</v>
       </c>
     </row>
-    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -6880,7 +6882,7 @@
         <v>9.3666666666666671</v>
       </c>
     </row>
-    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -6954,7 +6956,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -7028,7 +7030,7 @@
         <v>6.0333333333333332</v>
       </c>
     </row>
-    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>152</v>
       </c>
@@ -7102,7 +7104,7 @@
         <v>9.3666666666666671</v>
       </c>
     </row>
-    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -7176,7 +7178,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>115</v>
       </c>
@@ -7250,7 +7252,7 @@
         <v>4.0333333333333332</v>
       </c>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -7275,7 +7277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -7423,7 +7425,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -7497,7 +7499,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -7571,7 +7573,7 @@
         <v>7.3666666666666663</v>
       </c>
     </row>
-    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -7645,7 +7647,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -7719,7 +7721,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -7793,7 +7795,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -7867,7 +7869,7 @@
         <v>8.0333333333333332</v>
       </c>
     </row>
-    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>131</v>
       </c>
@@ -7941,7 +7943,7 @@
         <v>8.0333333333333332</v>
       </c>
     </row>
-    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -8015,7 +8017,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -8089,7 +8091,7 @@
         <v>3.3666666666666663</v>
       </c>
     </row>
-    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>145</v>
       </c>
@@ -8102,16 +8104,65 @@
       <c r="D44" t="s">
         <v>147</v>
       </c>
+      <c r="E44" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+      <c r="N44" s="1">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1">
+        <v>1</v>
+      </c>
+      <c r="P44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1">
+        <v>1</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1</v>
+      </c>
+      <c r="T44" s="1">
+        <v>1</v>
+      </c>
       <c r="U44" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V44" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.6666666666666661</v>
       </c>
       <c r="W44" s="4">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>7.3666666666666663</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -8188,7 +8239,7 @@
         <v>10.033333333333333</v>
       </c>
     </row>
-    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -8263,13 +8314,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A46" xr:uid="{282BE024-4F4F-468F-BFFD-FBEB26858532}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="SANCHEZ MARTINEZ XIMENA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="V2:W46">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
@@ -8285,11 +8329,11 @@
   <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7305" ySplit="900" topLeftCell="W5" activePane="bottomLeft"/>
+      <pane xSplit="7305" ySplit="900" topLeftCell="R32" activePane="bottomRight"/>
       <selection activeCell="A45" sqref="A45"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8474,30 +8518,30 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f>SUM(F3:I3)</f>
+        <f t="shared" ref="N3:N47" si="0">SUM(F3:I3)</f>
         <v>15</v>
       </c>
       <c r="O3" s="4">
-        <f>(N3/19)*10</f>
+        <f t="shared" ref="O3:O47" si="1">(N3/19)*10</f>
         <v>7.8947368421052637</v>
       </c>
       <c r="P3" s="1">
-        <f>SUM(J3:M3)</f>
+        <f t="shared" ref="P3:P47" si="2">SUM(J3:M3)</f>
         <v>0</v>
       </c>
       <c r="Q3" s="4">
-        <f>(P3/12)*10</f>
+        <f t="shared" ref="Q3:Q47" si="3">(P3/12)*10</f>
         <v>0</v>
       </c>
       <c r="R3" s="4">
-        <f>IF(O3+Q3&gt;10, 10, O3+Q3)</f>
+        <f t="shared" ref="R3:R47" si="4">IF(O3+Q3&gt;10, 10, O3+Q3)</f>
         <v>7.8947368421052637</v>
       </c>
       <c r="S3" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T3" s="4">
-        <f>SUM(R3,S3)/2</f>
+        <f t="shared" ref="T3:T47" si="5">SUM(R3,S3)/2</f>
         <v>7.6307017543859654</v>
       </c>
       <c r="U3" s="1">
@@ -8507,11 +8551,11 @@
         <v>8</v>
       </c>
       <c r="W3" s="4">
-        <f>SUM(U3:V3)/2</f>
+        <f t="shared" ref="W3:W47" si="6">SUM(U3:V3)/2</f>
         <v>8</v>
       </c>
       <c r="X3" s="4">
-        <f>T3*0.7+W3*0.3</f>
+        <f t="shared" ref="X3:X47" si="7">T3*0.7+W3*0.3</f>
         <v>7.741491228070176</v>
       </c>
       <c r="Y3" s="1">
@@ -8559,30 +8603,30 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <f>SUM(F4:I4)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="O4" s="4">
-        <f>(N4/19)*10</f>
+        <f t="shared" si="1"/>
         <v>6.8421052631578947</v>
       </c>
       <c r="P4" s="1">
-        <f>SUM(J4:M4)</f>
+        <f t="shared" si="2"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="Q4" s="4">
-        <f>(P4/12)*10</f>
+        <f t="shared" si="3"/>
         <v>2.125</v>
       </c>
       <c r="R4" s="4">
-        <f>IF(O4+Q4&gt;10, 10, O4+Q4)</f>
+        <f t="shared" si="4"/>
         <v>8.9671052631578938</v>
       </c>
       <c r="S4" s="4">
         <v>6.0333333333333332</v>
       </c>
       <c r="T4" s="4">
-        <f>SUM(R4,S4)/2</f>
+        <f t="shared" si="5"/>
         <v>7.5002192982456135</v>
       </c>
       <c r="U4" s="1">
@@ -8592,11 +8636,11 @@
         <v>9</v>
       </c>
       <c r="W4" s="4">
-        <f>SUM(U4:V4)/2</f>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="X4" s="4">
-        <f>T4*0.7+W4*0.3</f>
+        <f t="shared" si="7"/>
         <v>6.6001535087719292</v>
       </c>
       <c r="Y4" s="1">
@@ -8644,30 +8688,30 @@
         <v>1</v>
       </c>
       <c r="N5" s="1">
-        <f>SUM(F5:I5)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="O5" s="4">
-        <f>(N5/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.9473684210526319</v>
       </c>
       <c r="P5" s="1">
-        <f>SUM(J5:M5)</f>
+        <f t="shared" si="2"/>
         <v>9.25</v>
       </c>
       <c r="Q5" s="4">
-        <f>(P5/12)*10</f>
+        <f t="shared" si="3"/>
         <v>7.7083333333333339</v>
       </c>
       <c r="R5" s="4">
-        <f>IF(O5+Q5&gt;10, 10, O5+Q5)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S5" s="4">
         <v>8.0333333333333332</v>
       </c>
       <c r="T5" s="4">
-        <f>SUM(R5,S5)/2</f>
+        <f t="shared" si="5"/>
         <v>9.0166666666666657</v>
       </c>
       <c r="U5" s="1">
@@ -8677,11 +8721,11 @@
         <v>9</v>
       </c>
       <c r="W5" s="4">
-        <f>SUM(U5:V5)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X5" s="4">
-        <f>T5*0.7+W5*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.1616666666666653</v>
       </c>
       <c r="Y5" s="1">
@@ -8729,30 +8773,30 @@
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <f>SUM(F6:I6)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O6" s="4">
-        <f>(N6/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.473684210526315</v>
       </c>
       <c r="P6" s="1">
-        <f>SUM(J6:M6)</f>
+        <f t="shared" si="2"/>
         <v>3.35</v>
       </c>
       <c r="Q6" s="4">
-        <f>(P6/12)*10</f>
+        <f t="shared" si="3"/>
         <v>2.791666666666667</v>
       </c>
       <c r="R6" s="4">
-        <f>IF(O6+Q6&gt;10, 10, O6+Q6)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S6" s="4">
         <v>10.033333333333333</v>
       </c>
       <c r="T6" s="4">
-        <f>SUM(R6,S6)/2</f>
+        <f t="shared" si="5"/>
         <v>10.016666666666666</v>
       </c>
       <c r="U6" s="1">
@@ -8762,11 +8806,11 @@
         <v>0</v>
       </c>
       <c r="W6" s="4">
-        <f>SUM(U6:V6)/2</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="X6" s="4">
-        <f>T6*0.7+W6*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.5116666666666667</v>
       </c>
       <c r="Y6" s="1">
@@ -8814,30 +8858,30 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f>SUM(F7:I7)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="O7" s="4">
-        <f>(N7/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.2105263157894726</v>
       </c>
       <c r="P7" s="1">
-        <f>SUM(J7:M7)</f>
+        <f t="shared" si="2"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="Q7" s="4">
-        <f>(P7/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.9166666666666679</v>
       </c>
       <c r="R7" s="4">
-        <f>IF(O7+Q7&gt;10, 10, O7+Q7)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S7" s="4">
         <v>6</v>
       </c>
       <c r="T7" s="4">
-        <f>SUM(R7,S7)/2</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="U7" s="1">
@@ -8847,11 +8891,11 @@
         <v>8</v>
       </c>
       <c r="W7" s="4">
-        <f>SUM(U7:V7)/2</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="X7" s="4">
-        <f>T7*0.7+W7*0.3</f>
+        <f t="shared" si="7"/>
         <v>6.8</v>
       </c>
       <c r="Y7" s="1">
@@ -8899,30 +8943,30 @@
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <f>SUM(F8:I8)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="O8" s="4">
-        <f>(N8/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.2105263157894726</v>
       </c>
       <c r="P8" s="1">
-        <f>SUM(J8:M8)</f>
+        <f t="shared" si="2"/>
         <v>5.4</v>
       </c>
       <c r="Q8" s="4">
-        <f>(P8/12)*10</f>
+        <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
       <c r="R8" s="4">
-        <f>IF(O8+Q8&gt;10, 10, O8+Q8)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S8" s="4">
         <v>9.3666666666666671</v>
       </c>
       <c r="T8" s="4">
-        <f>SUM(R8,S8)/2</f>
+        <f t="shared" si="5"/>
         <v>9.6833333333333336</v>
       </c>
       <c r="U8" s="1">
@@ -8932,11 +8976,11 @@
         <v>10</v>
       </c>
       <c r="W8" s="4">
-        <f>SUM(U8:V8)/2</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="X8" s="4">
-        <f>T8*0.7+W8*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.2783333333333324</v>
       </c>
       <c r="Y8" s="1">
@@ -8984,30 +9028,30 @@
         <v>0.75</v>
       </c>
       <c r="N9" s="1">
-        <f>SUM(F9:I9)</f>
+        <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
       <c r="O9" s="4">
-        <f>(N9/19)*10</f>
+        <f t="shared" si="1"/>
         <v>7.6315789473684212</v>
       </c>
       <c r="P9" s="1">
-        <f>SUM(J9:M9)</f>
+        <f t="shared" si="2"/>
         <v>4.75</v>
       </c>
       <c r="Q9" s="4">
-        <f>(P9/12)*10</f>
+        <f t="shared" si="3"/>
         <v>3.958333333333333</v>
       </c>
       <c r="R9" s="4">
-        <f>IF(O9+Q9&gt;10, 10, O9+Q9)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S9" s="4">
         <v>5.3666666666666671</v>
       </c>
       <c r="T9" s="4">
-        <f>SUM(R9,S9)/2</f>
+        <f t="shared" si="5"/>
         <v>7.6833333333333336</v>
       </c>
       <c r="U9" s="1">
@@ -9017,11 +9061,11 @@
         <v>8</v>
       </c>
       <c r="W9" s="4">
-        <f>SUM(U9:V9)/2</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="X9" s="4">
-        <f>T9*0.7+W9*0.3</f>
+        <f t="shared" si="7"/>
         <v>6.5783333333333331</v>
       </c>
       <c r="Y9" s="1">
@@ -9069,30 +9113,30 @@
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f>SUM(F10:I10)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="O10" s="4">
-        <f>(N10/19)*10</f>
+        <f t="shared" si="1"/>
         <v>5.2631578947368416</v>
       </c>
       <c r="P10" s="1">
-        <f>SUM(J10:M10)</f>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="Q10" s="4">
-        <f>(P10/12)*10</f>
+        <f t="shared" si="3"/>
         <v>2.916666666666667</v>
       </c>
       <c r="R10" s="4">
-        <f>IF(O10+Q10&gt;10, 10, O10+Q10)</f>
+        <f t="shared" si="4"/>
         <v>8.1798245614035086</v>
       </c>
       <c r="S10" s="4">
         <v>8.0333333333333332</v>
       </c>
       <c r="T10" s="4">
-        <f>SUM(R10,S10)/2</f>
+        <f t="shared" si="5"/>
         <v>8.1065789473684209</v>
       </c>
       <c r="U10" s="1">
@@ -9102,11 +9146,11 @@
         <v>9</v>
       </c>
       <c r="W10" s="4">
-        <f>SUM(U10:V10)/2</f>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="X10" s="4">
-        <f>T10*0.7+W10*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.0246052631578939</v>
       </c>
       <c r="Y10" s="1">
@@ -9154,30 +9198,30 @@
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <f>SUM(F11:I11)</f>
+        <f t="shared" si="0"/>
         <v>18.25</v>
       </c>
       <c r="O11" s="4">
-        <f>(N11/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.6052631578947363</v>
       </c>
       <c r="P11" s="1">
-        <f>SUM(J11:M11)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="Q11" s="4">
-        <f>(P11/12)*10</f>
+        <f t="shared" si="3"/>
         <v>4.166666666666667</v>
       </c>
       <c r="R11" s="4">
-        <f>IF(O11+Q11&gt;10, 10, O11+Q11)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S11" s="4">
         <v>6.7</v>
       </c>
       <c r="T11" s="4">
-        <f>SUM(R11,S11)/2</f>
+        <f t="shared" si="5"/>
         <v>8.35</v>
       </c>
       <c r="U11" s="1">
@@ -9187,11 +9231,11 @@
         <v>9</v>
       </c>
       <c r="W11" s="4">
-        <f>SUM(U11:V11)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X11" s="4">
-        <f>T11*0.7+W11*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.5449999999999999</v>
       </c>
       <c r="Y11" s="1">
@@ -9239,30 +9283,30 @@
         <v>1</v>
       </c>
       <c r="N12" s="1">
-        <f>SUM(F12:I12)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="O12" s="4">
-        <f>(N12/19)*10</f>
+        <f t="shared" si="1"/>
         <v>7.8947368421052637</v>
       </c>
       <c r="P12" s="1">
-        <f>SUM(J12:M12)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q12" s="4">
-        <f>(P12/12)*10</f>
+        <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="R12" s="4">
-        <f>IF(O12+Q12&gt;10, 10, O12+Q12)</f>
+        <f t="shared" si="4"/>
         <v>9.5614035087719298</v>
       </c>
       <c r="S12" s="4">
         <v>4.7</v>
       </c>
       <c r="T12" s="4">
-        <f>SUM(R12,S12)/2</f>
+        <f t="shared" si="5"/>
         <v>7.1307017543859654</v>
       </c>
       <c r="U12" s="1">
@@ -9272,11 +9316,11 @@
         <v>0</v>
       </c>
       <c r="W12" s="4">
-        <f>SUM(U12:V12)/2</f>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="X12" s="4">
-        <f>T12*0.7+W12*0.3</f>
+        <f t="shared" si="7"/>
         <v>6.3414912280701747</v>
       </c>
       <c r="Y12" s="1">
@@ -9324,30 +9368,30 @@
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <f>SUM(F13:I13)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O13" s="4">
-        <f>(N13/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P13" s="1">
-        <f>SUM(J13:M13)</f>
+        <f t="shared" si="2"/>
         <v>4.8</v>
       </c>
       <c r="Q13" s="4">
-        <f>(P13/12)*10</f>
+        <f t="shared" si="3"/>
         <v>3.9999999999999996</v>
       </c>
       <c r="R13" s="4">
-        <f>IF(O13+Q13&gt;10, 10, O13+Q13)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S13" s="4">
         <v>6.7</v>
       </c>
       <c r="T13" s="4">
-        <f>SUM(R13,S13)/2</f>
+        <f t="shared" si="5"/>
         <v>8.35</v>
       </c>
       <c r="U13" s="1">
@@ -9357,11 +9401,11 @@
         <v>9</v>
       </c>
       <c r="W13" s="4">
-        <f>SUM(U13:V13)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X13" s="4">
-        <f>T13*0.7+W13*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.5449999999999999</v>
       </c>
       <c r="Y13" s="1">
@@ -9409,30 +9453,30 @@
         <v>0</v>
       </c>
       <c r="N14" s="1">
-        <f>SUM(F14:I14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O14" s="4">
-        <f>(N14/19)*10</f>
+        <f t="shared" si="1"/>
         <v>0.52631578947368418</v>
       </c>
       <c r="P14" s="1">
-        <f>SUM(J14:M14)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Q14" s="4">
-        <f>(P14/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.6666666666666661</v>
       </c>
       <c r="R14" s="4">
-        <f>IF(O14+Q14&gt;10, 10, O14+Q14)</f>
+        <f t="shared" si="4"/>
         <v>7.1929824561403501</v>
       </c>
       <c r="S14" s="4">
         <v>8.6999999999999993</v>
       </c>
       <c r="T14" s="4">
-        <f>SUM(R14,S14)/2</f>
+        <f t="shared" si="5"/>
         <v>7.9464912280701743</v>
       </c>
       <c r="U14" s="1">
@@ -9442,11 +9486,11 @@
         <v>0</v>
       </c>
       <c r="W14" s="4">
-        <f>SUM(U14:V14)/2</f>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="X14" s="4">
-        <f>T14*0.7+W14*0.3</f>
+        <f t="shared" si="7"/>
         <v>6.6125438596491213</v>
       </c>
       <c r="Y14" s="1">
@@ -9494,30 +9538,30 @@
         <v>1</v>
       </c>
       <c r="N15" s="1">
-        <f>SUM(F15:I15)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="O15" s="4">
-        <f>(N15/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.9473684210526319</v>
       </c>
       <c r="P15" s="1">
-        <f>SUM(J15:M15)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q15" s="4">
-        <f>(P15/12)*10</f>
+        <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="R15" s="4">
-        <f>IF(O15+Q15&gt;10, 10, O15+Q15)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S15" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T15" s="4">
-        <f>SUM(R15,S15)/2</f>
+        <f t="shared" si="5"/>
         <v>8.6833333333333336</v>
       </c>
       <c r="U15" s="1">
@@ -9527,11 +9571,11 @@
         <v>9</v>
       </c>
       <c r="W15" s="4">
-        <f>SUM(U15:V15)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X15" s="4">
-        <f>T15*0.7+W15*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.7783333333333324</v>
       </c>
       <c r="Y15" s="1">
@@ -9579,30 +9623,30 @@
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <f>SUM(F16:I16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O16" s="4">
-        <f>(N16/19)*10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" s="1">
-        <f>SUM(J16:M16)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q16" s="4">
-        <f>(P16/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="R16" s="4">
-        <f>IF(O16+Q16&gt;10, 10, O16+Q16)</f>
+        <f t="shared" si="4"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="S16" s="4">
         <v>6.7</v>
       </c>
       <c r="T16" s="4">
-        <f>SUM(R16,S16)/2</f>
+        <f t="shared" si="5"/>
         <v>3.7666666666666666</v>
       </c>
       <c r="U16" s="1">
@@ -9612,11 +9656,11 @@
         <v>0</v>
       </c>
       <c r="W16" s="4">
-        <f>SUM(U16:V16)/2</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X16" s="4">
-        <f>T16*0.7+W16*0.3</f>
+        <f t="shared" si="7"/>
         <v>2.6366666666666663</v>
       </c>
       <c r="Y16" s="1">
@@ -9664,30 +9708,30 @@
         <v>1</v>
       </c>
       <c r="N17" s="1">
-        <f>SUM(F17:I17)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="O17" s="4">
-        <f>(N17/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.4210526315789469</v>
       </c>
       <c r="P17" s="1">
-        <f>SUM(J17:M17)</f>
+        <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
       <c r="Q17" s="4">
-        <f>(P17/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.875</v>
       </c>
       <c r="R17" s="4">
-        <f>IF(O17+Q17&gt;10, 10, O17+Q17)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S17" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T17" s="4">
-        <f>SUM(R17,S17)/2</f>
+        <f t="shared" si="5"/>
         <v>8.6833333333333336</v>
       </c>
       <c r="U17" s="1">
@@ -9697,11 +9741,11 @@
         <v>0</v>
       </c>
       <c r="W17" s="4">
-        <f>SUM(U17:V17)/2</f>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="X17" s="4">
-        <f>T17*0.7+W17*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.4283333333333328</v>
       </c>
       <c r="Y17" s="1">
@@ -9749,30 +9793,30 @@
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <f>SUM(F18:I18)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="O18" s="4">
-        <f>(N18/19)*10</f>
+        <f t="shared" si="1"/>
         <v>4.4736842105263159</v>
       </c>
       <c r="P18" s="1">
-        <f>SUM(J18:M18)</f>
+        <f t="shared" si="2"/>
         <v>7.75</v>
       </c>
       <c r="Q18" s="4">
-        <f>(P18/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.4583333333333339</v>
       </c>
       <c r="R18" s="4">
-        <f>IF(O18+Q18&gt;10, 10, O18+Q18)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S18" s="4">
         <v>5.3666666666666671</v>
       </c>
       <c r="T18" s="4">
-        <f>SUM(R18,S18)/2</f>
+        <f t="shared" si="5"/>
         <v>7.6833333333333336</v>
       </c>
       <c r="U18" s="1">
@@ -9782,11 +9826,11 @@
         <v>8</v>
       </c>
       <c r="W18" s="4">
-        <f>SUM(U18:V18)/2</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="X18" s="4">
-        <f>T18*0.7+W18*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.7783333333333324</v>
       </c>
       <c r="Y18" s="1">
@@ -9834,30 +9878,30 @@
         <v>0</v>
       </c>
       <c r="N19" s="1">
-        <f>SUM(F19:I19)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="O19" s="4">
-        <f>(N19/19)*10</f>
+        <f t="shared" si="1"/>
         <v>3.1578947368421053</v>
       </c>
       <c r="P19" s="1">
-        <f>SUM(J19:M19)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Q19" s="4">
-        <f>(P19/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.6666666666666661</v>
       </c>
       <c r="R19" s="4">
-        <f>IF(O19+Q19&gt;10, 10, O19+Q19)</f>
+        <f t="shared" si="4"/>
         <v>9.8245614035087705</v>
       </c>
       <c r="S19" s="4">
         <v>10.033333333333333</v>
       </c>
       <c r="T19" s="4">
-        <f>SUM(R19,S19)/2</f>
+        <f t="shared" si="5"/>
         <v>9.9289473684210527</v>
       </c>
       <c r="U19" s="1">
@@ -9867,11 +9911,11 @@
         <v>0</v>
       </c>
       <c r="W19" s="4">
-        <f>SUM(U19:V19)/2</f>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="X19" s="4">
-        <f>T19*0.7+W19*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.0002631578947376</v>
       </c>
       <c r="Y19" s="1">
@@ -9919,30 +9963,30 @@
         <v>0</v>
       </c>
       <c r="N20" s="1">
-        <f>SUM(F20:I20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O20" s="4">
-        <f>(N20/19)*10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20" s="1">
-        <f>SUM(J20:M20)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q20" s="4">
-        <f>(P20/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R20" s="4">
-        <f>IF(O20+Q20&gt;10, 10, O20+Q20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S20" s="4">
         <v>0</v>
       </c>
       <c r="T20" s="4">
-        <f>SUM(R20,S20)/2</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U20" s="1">
@@ -9952,11 +9996,11 @@
         <v>0</v>
       </c>
       <c r="W20" s="4">
-        <f>SUM(U20:V20)/2</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X20" s="4">
-        <f>T20*0.7+W20*0.3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y20" s="1">
@@ -10004,30 +10048,30 @@
         <v>1</v>
       </c>
       <c r="N21" s="1">
-        <f>SUM(F21:I21)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="O21" s="4">
-        <f>(N21/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.2105263157894726</v>
       </c>
       <c r="P21" s="1">
-        <f>SUM(J21:M21)</f>
+        <f t="shared" si="2"/>
         <v>9.75</v>
       </c>
       <c r="Q21" s="4">
-        <f>(P21/12)*10</f>
+        <f t="shared" si="3"/>
         <v>8.125</v>
       </c>
       <c r="R21" s="4">
-        <f>IF(O21+Q21&gt;10, 10, O21+Q21)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S21" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T21" s="4">
-        <f>SUM(R21,S21)/2</f>
+        <f t="shared" si="5"/>
         <v>8.6833333333333336</v>
       </c>
       <c r="U21" s="1">
@@ -10037,11 +10081,11 @@
         <v>9</v>
       </c>
       <c r="W21" s="4">
-        <f>SUM(U21:V21)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X21" s="4">
-        <f>T21*0.7+W21*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.9283333333333328</v>
       </c>
       <c r="Y21" s="1">
@@ -10089,30 +10133,30 @@
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <f>SUM(F22:I22)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="O22" s="4">
-        <f>(N22/19)*10</f>
+        <f t="shared" si="1"/>
         <v>5.7894736842105265</v>
       </c>
       <c r="P22" s="1">
-        <f>SUM(J22:M22)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q22" s="4">
-        <f>(P22/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="R22" s="4">
-        <f>IF(O22+Q22&gt;10, 10, O22+Q22)</f>
+        <f t="shared" si="4"/>
         <v>6.6228070175438596</v>
       </c>
       <c r="S22" s="4">
         <v>2.7</v>
       </c>
       <c r="T22" s="4">
-        <f>SUM(R22,S22)/2</f>
+        <f t="shared" si="5"/>
         <v>4.6614035087719294</v>
       </c>
       <c r="U22" s="1">
@@ -10122,11 +10166,11 @@
         <v>9</v>
       </c>
       <c r="W22" s="4">
-        <f>SUM(U22:V22)/2</f>
+        <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
       <c r="X22" s="4">
-        <f>T22*0.7+W22*0.3</f>
+        <f t="shared" si="7"/>
         <v>5.8129824561403503</v>
       </c>
       <c r="Y22" s="1">
@@ -10174,30 +10218,30 @@
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <f>SUM(F23:I23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O23" s="4">
-        <f>(N23/19)*10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P23" s="1">
-        <f>SUM(J23:M23)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q23" s="4">
-        <f>(P23/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R23" s="4">
-        <f>IF(O23+Q23&gt;10, 10, O23+Q23)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S23" s="4">
         <v>9.3666666666666671</v>
       </c>
       <c r="T23" s="4">
-        <f>SUM(R23,S23)/2</f>
+        <f t="shared" si="5"/>
         <v>4.6833333333333336</v>
       </c>
       <c r="U23" s="1">
@@ -10207,11 +10251,11 @@
         <v>0</v>
       </c>
       <c r="W23" s="4">
-        <f>SUM(U23:V23)/2</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X23" s="4">
-        <f>T23*0.7+W23*0.3</f>
+        <f t="shared" si="7"/>
         <v>3.2783333333333333</v>
       </c>
       <c r="Y23" s="1">
@@ -10259,30 +10303,30 @@
         <v>1</v>
       </c>
       <c r="N24" s="1">
-        <f>SUM(F24:I24)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O24" s="4">
-        <f>(N24/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.473684210526315</v>
       </c>
       <c r="P24" s="1">
-        <f>SUM(J24:M24)</f>
+        <f t="shared" si="2"/>
         <v>9.75</v>
       </c>
       <c r="Q24" s="4">
-        <f>(P24/12)*10</f>
+        <f t="shared" si="3"/>
         <v>8.125</v>
       </c>
       <c r="R24" s="4">
-        <f>IF(O24+Q24&gt;10, 10, O24+Q24)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S24" s="4">
         <v>8.6999999999999993</v>
       </c>
       <c r="T24" s="4">
-        <f>SUM(R24,S24)/2</f>
+        <f t="shared" si="5"/>
         <v>9.35</v>
       </c>
       <c r="U24" s="1">
@@ -10292,11 +10336,11 @@
         <v>9</v>
       </c>
       <c r="W24" s="4">
-        <f>SUM(U24:V24)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X24" s="4">
-        <f>T24*0.7+W24*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.3949999999999996</v>
       </c>
       <c r="Y24" s="1">
@@ -10344,30 +10388,30 @@
         <v>1</v>
       </c>
       <c r="N25" s="1">
-        <f>SUM(F25:I25)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O25" s="4">
-        <f>(N25/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P25" s="1">
-        <f>SUM(J25:M25)</f>
+        <f t="shared" si="2"/>
         <v>9.4499999999999993</v>
       </c>
       <c r="Q25" s="4">
-        <f>(P25/12)*10</f>
+        <f t="shared" si="3"/>
         <v>7.875</v>
       </c>
       <c r="R25" s="4">
-        <f>IF(O25+Q25&gt;10, 10, O25+Q25)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S25" s="4">
         <v>8.0333333333333332</v>
       </c>
       <c r="T25" s="4">
-        <f>SUM(R25,S25)/2</f>
+        <f t="shared" si="5"/>
         <v>9.0166666666666657</v>
       </c>
       <c r="U25" s="1">
@@ -10377,11 +10421,11 @@
         <v>9</v>
       </c>
       <c r="W25" s="4">
-        <f>SUM(U25:V25)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X25" s="4">
-        <f>T25*0.7+W25*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.1616666666666653</v>
       </c>
       <c r="Y25" s="1">
@@ -10429,30 +10473,30 @@
         <v>1</v>
       </c>
       <c r="N26" s="1">
-        <f>SUM(F26:I26)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O26" s="4">
-        <f>(N26/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.473684210526315</v>
       </c>
       <c r="P26" s="1">
-        <f>SUM(J26:M26)</f>
+        <f t="shared" si="2"/>
         <v>5.7</v>
       </c>
       <c r="Q26" s="4">
-        <f>(P26/12)*10</f>
+        <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
       <c r="R26" s="4">
-        <f>IF(O26+Q26&gt;10, 10, O26+Q26)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S26" s="4">
         <v>8.6999999999999993</v>
       </c>
       <c r="T26" s="4">
-        <f>SUM(R26,S26)/2</f>
+        <f t="shared" si="5"/>
         <v>9.35</v>
       </c>
       <c r="U26" s="1">
@@ -10462,11 +10506,11 @@
         <v>9</v>
       </c>
       <c r="W26" s="4">
-        <f>SUM(U26:V26)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X26" s="4">
-        <f>T26*0.7+W26*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.3949999999999996</v>
       </c>
       <c r="Y26" s="1">
@@ -10514,30 +10558,30 @@
         <v>1</v>
       </c>
       <c r="N27" s="1">
-        <f>SUM(F27:I27)</f>
+        <f t="shared" si="0"/>
         <v>16.5</v>
       </c>
       <c r="O27" s="4">
-        <f>(N27/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.6842105263157894</v>
       </c>
       <c r="P27" s="1">
-        <f>SUM(J27:M27)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q27" s="4">
-        <f>(P27/12)*10</f>
+        <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="R27" s="4">
-        <f>IF(O27+Q27&gt;10, 10, O27+Q27)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S27" s="4">
         <v>9.3666666666666671</v>
       </c>
       <c r="T27" s="4">
-        <f>SUM(R27,S27)/2</f>
+        <f t="shared" si="5"/>
         <v>9.6833333333333336</v>
       </c>
       <c r="U27" s="1">
@@ -10547,11 +10591,11 @@
         <v>9</v>
       </c>
       <c r="W27" s="4">
-        <f>SUM(U27:V27)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X27" s="4">
-        <f>T27*0.7+W27*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.4783333333333335</v>
       </c>
       <c r="Y27" s="1">
@@ -10599,30 +10643,30 @@
         <v>1</v>
       </c>
       <c r="N28" s="1">
-        <f>SUM(F28:I28)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O28" s="4">
-        <f>(N28/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P28" s="1">
-        <f>SUM(J28:M28)</f>
+        <f t="shared" si="2"/>
         <v>10.8</v>
       </c>
       <c r="Q28" s="4">
-        <f>(P28/12)*10</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="R28" s="4">
-        <f>IF(O28+Q28&gt;10, 10, O28+Q28)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S28" s="4">
         <v>6.0333333333333332</v>
       </c>
       <c r="T28" s="4">
-        <f>SUM(R28,S28)/2</f>
+        <f t="shared" si="5"/>
         <v>8.0166666666666657</v>
       </c>
       <c r="U28" s="1">
@@ -10632,11 +10676,11 @@
         <v>9</v>
       </c>
       <c r="W28" s="4">
-        <f>SUM(U28:V28)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X28" s="4">
-        <f>T28*0.7+W28*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.461666666666666</v>
       </c>
       <c r="Y28" s="1">
@@ -10684,30 +10728,30 @@
         <v>1</v>
       </c>
       <c r="N29" s="1">
-        <f>SUM(F29:I29)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O29" s="4">
-        <f>(N29/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.473684210526315</v>
       </c>
       <c r="P29" s="1">
-        <f>SUM(J29:M29)</f>
+        <f t="shared" si="2"/>
         <v>9.25</v>
       </c>
       <c r="Q29" s="4">
-        <f>(P29/12)*10</f>
+        <f t="shared" si="3"/>
         <v>7.7083333333333339</v>
       </c>
       <c r="R29" s="4">
-        <f>IF(O29+Q29&gt;10, 10, O29+Q29)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S29" s="4">
         <v>10.033333333333333</v>
       </c>
       <c r="T29" s="4">
-        <f>SUM(R29,S29)/2</f>
+        <f t="shared" si="5"/>
         <v>10.016666666666666</v>
       </c>
       <c r="U29" s="1">
@@ -10717,11 +10761,11 @@
         <v>8</v>
       </c>
       <c r="W29" s="4">
-        <f>SUM(U29:V29)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X29" s="4">
-        <f>T29*0.7+W29*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.711666666666666</v>
       </c>
       <c r="Y29" s="1">
@@ -10769,30 +10813,30 @@
         <v>1</v>
       </c>
       <c r="N30" s="1">
-        <f>SUM(F30:I30)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="O30" s="4">
-        <f>(N30/19)*10</f>
+        <f t="shared" si="1"/>
         <v>6.3157894736842106</v>
       </c>
       <c r="P30" s="1">
-        <f>SUM(J30:M30)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Q30" s="4">
-        <f>(P30/12)*10</f>
+        <f t="shared" si="3"/>
         <v>3.333333333333333</v>
       </c>
       <c r="R30" s="4">
-        <f>IF(O30+Q30&gt;10, 10, O30+Q30)</f>
+        <f t="shared" si="4"/>
         <v>9.6491228070175445</v>
       </c>
       <c r="S30" s="4">
         <v>9.3666666666666671</v>
       </c>
       <c r="T30" s="4">
-        <f>SUM(R30,S30)/2</f>
+        <f t="shared" si="5"/>
         <v>9.5078947368421058</v>
       </c>
       <c r="U30" s="1">
@@ -10802,11 +10846,11 @@
         <v>9</v>
       </c>
       <c r="W30" s="4">
-        <f>SUM(U30:V30)/2</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="X30" s="4">
-        <f>T30*0.7+W30*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.0555263157894732</v>
       </c>
       <c r="Y30" s="1">
@@ -10854,30 +10898,30 @@
         <v>0</v>
       </c>
       <c r="N31" s="1">
-        <f>SUM(F31:I31)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O31" s="4">
-        <f>(N31/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.473684210526315</v>
       </c>
       <c r="P31" s="1">
-        <f>SUM(J31:M31)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="Q31" s="4">
-        <f>(P31/12)*10</f>
+        <f t="shared" si="3"/>
         <v>4.166666666666667</v>
       </c>
       <c r="R31" s="4">
-        <f>IF(O31+Q31&gt;10, 10, O31+Q31)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S31" s="4">
         <v>5.3666666666666671</v>
       </c>
       <c r="T31" s="4">
-        <f>SUM(R31,S31)/2</f>
+        <f t="shared" si="5"/>
         <v>7.6833333333333336</v>
       </c>
       <c r="U31" s="1">
@@ -10887,11 +10931,11 @@
         <v>10</v>
       </c>
       <c r="W31" s="4">
-        <f>SUM(U31:V31)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X31" s="4">
-        <f>T31*0.7+W31*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.2283333333333335</v>
       </c>
       <c r="Y31" s="1">
@@ -10939,30 +10983,30 @@
         <v>1</v>
       </c>
       <c r="N32" s="1">
-        <f>SUM(F32:I32)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="O32" s="4">
-        <f>(N32/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.2105263157894726</v>
       </c>
       <c r="P32" s="1">
-        <f>SUM(J32:M32)</f>
+        <f t="shared" si="2"/>
         <v>11.25</v>
       </c>
       <c r="Q32" s="4">
-        <f>(P32/12)*10</f>
+        <f t="shared" si="3"/>
         <v>9.375</v>
       </c>
       <c r="R32" s="4">
-        <f>IF(O32+Q32&gt;10, 10, O32+Q32)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S32" s="4">
         <v>5.3666666666666671</v>
       </c>
       <c r="T32" s="4">
-        <f>SUM(R32,S32)/2</f>
+        <f t="shared" si="5"/>
         <v>7.6833333333333336</v>
       </c>
       <c r="U32" s="1">
@@ -10972,11 +11016,11 @@
         <v>10</v>
       </c>
       <c r="W32" s="4">
-        <f>SUM(U32:V32)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X32" s="4">
-        <f>T32*0.7+W32*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.2283333333333335</v>
       </c>
       <c r="Y32" s="1">
@@ -11024,30 +11068,30 @@
         <v>0</v>
       </c>
       <c r="N33" s="1">
-        <f>SUM(F33:I33)</f>
+        <f t="shared" si="0"/>
         <v>16.5</v>
       </c>
       <c r="O33" s="4">
-        <f>(N33/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.6842105263157894</v>
       </c>
       <c r="P33" s="1">
-        <f>SUM(J33:M33)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q33" s="4">
-        <f>(P33/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R33" s="4">
-        <f>IF(O33+Q33&gt;10, 10, O33+Q33)</f>
+        <f t="shared" si="4"/>
         <v>8.6842105263157894</v>
       </c>
       <c r="S33" s="4">
         <v>4.7</v>
       </c>
       <c r="T33" s="4">
-        <f>SUM(R33,S33)/2</f>
+        <f t="shared" si="5"/>
         <v>6.6921052631578952</v>
       </c>
       <c r="U33" s="1">
@@ -11057,11 +11101,11 @@
         <v>9</v>
       </c>
       <c r="W33" s="4">
-        <f>SUM(U33:V33)/2</f>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="X33" s="4">
-        <f>T33*0.7+W33*0.3</f>
+        <f t="shared" si="7"/>
         <v>6.0344736842105258</v>
       </c>
       <c r="Y33" s="1">
@@ -11109,30 +11153,30 @@
         <v>1</v>
       </c>
       <c r="N34" s="1">
-        <f>SUM(F34:I34)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O34" s="4">
-        <f>(N34/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P34" s="1">
-        <f>SUM(J34:M34)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q34" s="4">
-        <f>(P34/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="R34" s="4">
-        <f>IF(O34+Q34&gt;10, 10, O34+Q34)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S34" s="4">
         <v>4.0333333333333332</v>
       </c>
       <c r="T34" s="4">
-        <f>SUM(R34,S34)/2</f>
+        <f t="shared" si="5"/>
         <v>7.0166666666666666</v>
       </c>
       <c r="U34" s="1">
@@ -11142,11 +11186,11 @@
         <v>9</v>
       </c>
       <c r="W34" s="4">
-        <f>SUM(U34:V34)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X34" s="4">
-        <f>T34*0.7+W34*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.7616666666666667</v>
       </c>
       <c r="Y34" s="1">
@@ -11194,30 +11238,30 @@
         <v>1</v>
       </c>
       <c r="N35" s="1">
-        <f>SUM(F35:I35)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O35" s="4">
-        <f>(N35/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P35" s="1">
-        <f>SUM(J35:M35)</f>
+        <f t="shared" si="2"/>
         <v>8.9499999999999993</v>
       </c>
       <c r="Q35" s="4">
-        <f>(P35/12)*10</f>
+        <f t="shared" si="3"/>
         <v>7.4583333333333321</v>
       </c>
       <c r="R35" s="4">
-        <f>IF(O35+Q35&gt;10, 10, O35+Q35)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S35" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T35" s="4">
-        <f>SUM(R35,S35)/2</f>
+        <f t="shared" si="5"/>
         <v>8.6833333333333336</v>
       </c>
       <c r="U35" s="1">
@@ -11227,11 +11271,11 @@
         <v>9</v>
       </c>
       <c r="W35" s="4">
-        <f>SUM(U35:V35)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X35" s="4">
-        <f>T35*0.7+W35*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.7783333333333324</v>
       </c>
       <c r="Y35" s="1">
@@ -11279,30 +11323,30 @@
         <v>1</v>
       </c>
       <c r="N36" s="1">
-        <f>SUM(F36:I36)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O36" s="4">
-        <f>(N36/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P36" s="1">
-        <f>SUM(J36:M36)</f>
+        <f t="shared" si="2"/>
         <v>9.75</v>
       </c>
       <c r="Q36" s="4">
-        <f>(P36/12)*10</f>
+        <f t="shared" si="3"/>
         <v>8.125</v>
       </c>
       <c r="R36" s="4">
-        <f>IF(O36+Q36&gt;10, 10, O36+Q36)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S36" s="4">
         <v>3.3666666666666663</v>
       </c>
       <c r="T36" s="4">
-        <f>SUM(R36,S36)/2</f>
+        <f t="shared" si="5"/>
         <v>6.6833333333333336</v>
       </c>
       <c r="U36" s="1">
@@ -11312,11 +11356,11 @@
         <v>10</v>
       </c>
       <c r="W36" s="4">
-        <f>SUM(U36:V36)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X36" s="4">
-        <f>T36*0.7+W36*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.5283333333333324</v>
       </c>
       <c r="Y36" s="1">
@@ -11364,30 +11408,30 @@
         <v>1</v>
       </c>
       <c r="N37" s="1">
-        <f>SUM(F37:I37)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O37" s="4">
-        <f>(N37/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.473684210526315</v>
       </c>
       <c r="P37" s="1">
-        <f>SUM(J37:M37)</f>
+        <f t="shared" si="2"/>
         <v>5.3</v>
       </c>
       <c r="Q37" s="4">
-        <f>(P37/12)*10</f>
+        <f t="shared" si="3"/>
         <v>4.4166666666666661</v>
       </c>
       <c r="R37" s="4">
-        <f>IF(O37+Q37&gt;10, 10, O37+Q37)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S37" s="4">
         <v>10.033333333333333</v>
       </c>
       <c r="T37" s="4">
-        <f>SUM(R37,S37)/2</f>
+        <f t="shared" si="5"/>
         <v>10.016666666666666</v>
       </c>
       <c r="U37" s="1">
@@ -11397,11 +11441,11 @@
         <v>10</v>
       </c>
       <c r="W37" s="4">
-        <f>SUM(U37:V37)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X37" s="4">
-        <f>T37*0.7+W37*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.8616666666666664</v>
       </c>
       <c r="Y37" s="1">
@@ -11449,30 +11493,30 @@
         <v>0</v>
       </c>
       <c r="N38" s="1">
-        <f>SUM(F38:I38)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="O38" s="4">
-        <f>(N38/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.8157894736842106</v>
       </c>
       <c r="P38" s="1">
-        <f>SUM(J38:M38)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q38" s="4">
-        <f>(P38/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R38" s="4">
-        <f>IF(O38+Q38&gt;10, 10, O38+Q38)</f>
+        <f t="shared" si="4"/>
         <v>8.8157894736842106</v>
       </c>
       <c r="S38" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T38" s="4">
-        <f>SUM(R38,S38)/2</f>
+        <f t="shared" si="5"/>
         <v>8.091228070175438</v>
       </c>
       <c r="U38" s="1">
@@ -11482,11 +11526,11 @@
         <v>9</v>
       </c>
       <c r="W38" s="4">
-        <f>SUM(U38:V38)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X38" s="4">
-        <f>T38*0.7+W38*0.3</f>
+        <f t="shared" si="7"/>
         <v>8.5138596491228071</v>
       </c>
       <c r="Y38" s="1">
@@ -11534,30 +11578,30 @@
         <v>0</v>
       </c>
       <c r="N39" s="1">
-        <f>SUM(F39:I39)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="O39" s="4">
-        <f>(N39/19)*10</f>
+        <f t="shared" si="1"/>
         <v>2.6315789473684208</v>
       </c>
       <c r="P39" s="1">
-        <f>SUM(J39:M39)</f>
+        <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
       <c r="Q39" s="4">
-        <f>(P39/12)*10</f>
+        <f t="shared" si="3"/>
         <v>4.583333333333333</v>
       </c>
       <c r="R39" s="4">
-        <f>IF(O39+Q39&gt;10, 10, O39+Q39)</f>
+        <f t="shared" si="4"/>
         <v>7.2149122807017534</v>
       </c>
       <c r="S39" s="4">
         <v>8.0333333333333332</v>
       </c>
       <c r="T39" s="4">
-        <f>SUM(R39,S39)/2</f>
+        <f t="shared" si="5"/>
         <v>7.6241228070175433</v>
       </c>
       <c r="U39" s="1">
@@ -11567,11 +11611,11 @@
         <v>7</v>
       </c>
       <c r="W39" s="4">
-        <f>SUM(U39:V39)/2</f>
+        <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
       <c r="X39" s="4">
-        <f>T39*0.7+W39*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.2868859649122806</v>
       </c>
       <c r="Y39" s="1">
@@ -11619,30 +11663,30 @@
         <v>1</v>
       </c>
       <c r="N40" s="1">
-        <f>SUM(F40:I40)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="O40" s="4">
-        <f>(N40/19)*10</f>
+        <f t="shared" si="1"/>
         <v>8.9473684210526319</v>
       </c>
       <c r="P40" s="1">
-        <f>SUM(J40:M40)</f>
+        <f t="shared" si="2"/>
         <v>4.25</v>
       </c>
       <c r="Q40" s="4">
-        <f>(P40/12)*10</f>
+        <f t="shared" si="3"/>
         <v>3.541666666666667</v>
       </c>
       <c r="R40" s="4">
-        <f>IF(O40+Q40&gt;10, 10, O40+Q40)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S40" s="4">
         <v>10</v>
       </c>
       <c r="T40" s="4">
-        <f>SUM(R40,S40)/2</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="U40" s="1">
@@ -11652,11 +11696,11 @@
         <v>9</v>
       </c>
       <c r="W40" s="4">
-        <f>SUM(U40:V40)/2</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="X40" s="4">
-        <f>T40*0.7+W40*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.6999999999999993</v>
       </c>
       <c r="Y40" s="1">
@@ -11704,30 +11748,30 @@
         <v>0</v>
       </c>
       <c r="N41" s="1">
-        <f>SUM(F41:I41)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O41" s="4">
-        <f>(N41/19)*10</f>
+        <f t="shared" si="1"/>
         <v>0.52631578947368418</v>
       </c>
       <c r="P41" s="1">
-        <f>SUM(J41:M41)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q41" s="4">
-        <f>(P41/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R41" s="4">
-        <f>IF(O41+Q41&gt;10, 10, O41+Q41)</f>
+        <f t="shared" si="4"/>
         <v>0.52631578947368418</v>
       </c>
       <c r="S41" s="4">
         <v>7.3666666666666663</v>
       </c>
       <c r="T41" s="4">
-        <f>SUM(R41,S41)/2</f>
+        <f t="shared" si="5"/>
         <v>3.9464912280701752</v>
       </c>
       <c r="U41" s="1">
@@ -11737,11 +11781,11 @@
         <v>0</v>
       </c>
       <c r="W41" s="4">
-        <f>SUM(U41:V41)/2</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X41" s="4">
-        <f>T41*0.7+W41*0.3</f>
+        <f t="shared" si="7"/>
         <v>2.7625438596491225</v>
       </c>
       <c r="Y41" s="1">
@@ -11789,30 +11833,30 @@
         <v>1</v>
       </c>
       <c r="N42" s="1">
-        <f>SUM(F42:I42)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="O42" s="4">
-        <f>(N42/19)*10</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="P42" s="1">
-        <f>SUM(J42:M42)</f>
+        <f t="shared" si="2"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="Q42" s="4">
-        <f>(P42/12)*10</f>
+        <f t="shared" si="3"/>
         <v>7.3333333333333339</v>
       </c>
       <c r="R42" s="4">
-        <f>IF(O42+Q42&gt;10, 10, O42+Q42)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S42" s="4">
         <v>10</v>
       </c>
       <c r="T42" s="4">
-        <f>SUM(R42,S42)/2</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="U42" s="1">
@@ -11822,11 +11866,11 @@
         <v>10</v>
       </c>
       <c r="W42" s="4">
-        <f>SUM(U42:V42)/2</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="X42" s="4">
-        <f>T42*0.7+W42*0.3</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="Y42" s="1">
@@ -11874,30 +11918,30 @@
         <v>0</v>
       </c>
       <c r="N43" s="1">
-        <f>SUM(F43:I43)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="O43" s="4">
-        <f>(N43/19)*10</f>
+        <f t="shared" si="1"/>
         <v>7.8947368421052637</v>
       </c>
       <c r="P43" s="1">
-        <f>SUM(J43:M43)</f>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="Q43" s="4">
-        <f>(P43/12)*10</f>
+        <f t="shared" si="3"/>
         <v>2.916666666666667</v>
       </c>
       <c r="R43" s="4">
-        <f>IF(O43+Q43&gt;10, 10, O43+Q43)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S43" s="4">
         <v>8.6999999999999993</v>
       </c>
       <c r="T43" s="4">
-        <f>SUM(R43,S43)/2</f>
+        <f t="shared" si="5"/>
         <v>9.35</v>
       </c>
       <c r="U43" s="1">
@@ -11907,11 +11951,11 @@
         <v>8</v>
       </c>
       <c r="W43" s="4">
-        <f>SUM(U43:V43)/2</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="X43" s="4">
-        <f>T43*0.7+W43*0.3</f>
+        <f t="shared" si="7"/>
         <v>7.7449999999999992</v>
       </c>
       <c r="Y43" s="1">
@@ -11959,31 +12003,31 @@
         <v>1</v>
       </c>
       <c r="N44" s="1">
-        <f>SUM(F44:I44)</f>
+        <f t="shared" si="0"/>
         <v>12.8</v>
       </c>
       <c r="O44" s="4">
-        <f>(N44/19)*10</f>
+        <f t="shared" si="1"/>
         <v>6.7368421052631575</v>
       </c>
       <c r="P44" s="1">
-        <f>SUM(J44:M44)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Q44" s="4">
-        <f>(P44/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.6666666666666661</v>
       </c>
       <c r="R44" s="4">
-        <f>IF(O44+Q44&gt;10, 10, O44+Q44)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S44" s="4">
-        <v>0</v>
+        <v>7.4</v>
       </c>
       <c r="T44" s="4">
-        <f>SUM(R44,S44)/2</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>8.6999999999999993</v>
       </c>
       <c r="U44" s="1">
         <v>0</v>
@@ -11992,12 +12036,12 @@
         <v>0</v>
       </c>
       <c r="W44" s="4">
-        <f>SUM(U44:V44)/2</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X44" s="4">
-        <f>T44*0.7+W44*0.3</f>
-        <v>3.5</v>
+        <f t="shared" si="7"/>
+        <v>6.089999999999999</v>
       </c>
       <c r="Y44" s="1">
         <v>3</v>
@@ -12044,30 +12088,30 @@
         <v>1</v>
       </c>
       <c r="N45" s="1">
-        <f>SUM(F45:I45)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="O45" s="4">
-        <f>(N45/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.2105263157894726</v>
       </c>
       <c r="P45" s="1">
-        <f>SUM(J45:M45)</f>
+        <f t="shared" si="2"/>
         <v>9.75</v>
       </c>
       <c r="Q45" s="4">
-        <f>(P45/12)*10</f>
+        <f t="shared" si="3"/>
         <v>8.125</v>
       </c>
       <c r="R45" s="4">
-        <f>IF(O45+Q45&gt;10, 10, O45+Q45)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S45" s="4">
         <v>9.3666666666666671</v>
       </c>
       <c r="T45" s="4">
-        <f>SUM(R45,S45)/2</f>
+        <f t="shared" si="5"/>
         <v>9.6833333333333336</v>
       </c>
       <c r="U45" s="1">
@@ -12077,11 +12121,11 @@
         <v>9</v>
       </c>
       <c r="W45" s="4">
-        <f>SUM(U45:V45)/2</f>
+        <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
       <c r="X45" s="4">
-        <f>T45*0.7+W45*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.6283333333333339</v>
       </c>
       <c r="Y45" s="1">
@@ -12129,30 +12173,30 @@
         <v>0</v>
       </c>
       <c r="N46" s="1">
-        <f>SUM(F46:I46)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="O46" s="4">
-        <f>(N46/19)*10</f>
+        <f t="shared" si="1"/>
         <v>9.7368421052631575</v>
       </c>
       <c r="P46" s="1">
-        <f>SUM(J46:M46)</f>
+        <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
       <c r="Q46" s="4">
-        <f>(P46/12)*10</f>
+        <f t="shared" si="3"/>
         <v>6.875</v>
       </c>
       <c r="R46" s="4">
-        <f>IF(O46+Q46&gt;10, 10, O46+Q46)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="S46" s="4">
         <v>9.3666666666666671</v>
       </c>
       <c r="T46" s="4">
-        <f>SUM(R46,S46)/2</f>
+        <f t="shared" si="5"/>
         <v>9.6833333333333336</v>
       </c>
       <c r="U46" s="1">
@@ -12162,11 +12206,11 @@
         <v>10</v>
       </c>
       <c r="W46" s="4">
-        <f>SUM(U46:V46)/2</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="X46" s="4">
-        <f>T46*0.7+W46*0.3</f>
+        <f t="shared" si="7"/>
         <v>9.7783333333333324</v>
       </c>
       <c r="Y46" s="1">
@@ -12214,45 +12258,45 @@
         <v>0</v>
       </c>
       <c r="N47" s="1">
-        <f>SUM(F47:I47)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="O47" s="4">
-        <f>(N47/19)*10</f>
+        <f t="shared" si="1"/>
         <v>7.8947368421052637</v>
       </c>
       <c r="P47" s="1">
-        <f>SUM(J47:M47)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q47" s="4">
-        <f>(P47/12)*10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R47" s="4">
-        <f>IF(O47+Q47&gt;10, 10, O47+Q47)</f>
+        <f t="shared" si="4"/>
         <v>7.8947368421052637</v>
       </c>
       <c r="S47" s="4">
         <v>8.0333333333333332</v>
       </c>
       <c r="T47" s="4">
-        <f>SUM(R47,S47)/2</f>
+        <f t="shared" si="5"/>
         <v>7.9640350877192985</v>
       </c>
       <c r="U47" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V47" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W47" s="4">
-        <f>SUM(U47:V47)/2</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="X47" s="4">
-        <f>T47*0.7+W47*0.3</f>
-        <v>5.574824561403509</v>
+        <f t="shared" si="7"/>
+        <v>8.2748245614035092</v>
       </c>
       <c r="Y47" s="1">
         <v>0</v>

</xml_diff>